<commit_message>
Add input file pattern support (e.g. Folder/*.xls*)
</commit_message>
<xml_diff>
--- a/Performer/Config.xlsx
+++ b/Performer/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60BB3261-0CBC-498D-8310-37829ABB9211}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -53,12 +54,6 @@
     <t>AppFilePath</t>
   </si>
   <si>
-    <t>Errors</t>
-  </si>
-  <si>
-    <t>C:\WINDOWS\system32\notepad.exe</t>
-  </si>
-  <si>
     <t>OpenApps</t>
   </si>
   <si>
@@ -86,12 +81,6 @@
     <t>TempFolder</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>InputFile</t>
-  </si>
-  <si>
     <t>Sample data for running the template</t>
   </si>
   <si>
@@ -227,12 +216,6 @@
     <t>RFW-Login</t>
   </si>
   <si>
-    <t>..\TestData\Sample1.xlsx</t>
-  </si>
-  <si>
-    <t>../TestData/Output/[File]</t>
-  </si>
-  <si>
     <t>../TestData</t>
   </si>
   <si>
@@ -281,13 +264,34 @@
     <t>Test ReFrameWork</t>
   </si>
   <si>
-    <t>../TestData/Processed</t>
+    <t>InputPath</t>
+  </si>
+  <si>
+    <t>Archive folder path for processed files</t>
+  </si>
+  <si>
+    <t>../TestData/Temp/[File]</t>
+  </si>
+  <si>
+    <t>../TestData/Output</t>
+  </si>
+  <si>
+    <t>C:/WINDOWS/system32/notepad.exe</t>
+  </si>
+  <si>
+    <t>../TestData/Errors</t>
+  </si>
+  <si>
+    <t>../TestData/Temp</t>
+  </si>
+  <si>
+    <t>../TestData/*.xls*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -678,11 +682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -705,13 +709,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -722,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -743,24 +747,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -768,21 +772,21 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -790,49 +794,60 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
     </row>
   </sheetData>
@@ -842,7 +857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -861,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -873,7 +888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -889,7 +904,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -900,13 +915,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -916,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -943,13 +958,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -965,123 +980,123 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
         <v>84</v>
       </c>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -1089,60 +1104,60 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1"/>
-    <hyperlink ref="B22" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B22" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add an asset to facilitate switching environments assets and queues
</commit_message>
<xml_diff>
--- a/Performer/Config.xlsx
+++ b/Performer/Config.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60BB3261-0CBC-498D-8310-37829ABB9211}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C2B6A93D-8C52-4CB9-95C5-42970E86037C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10260" windowHeight="10703" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -286,6 +286,21 @@
   </si>
   <si>
     <t>../TestData/*.xls*</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>RFW-Environment</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>RFW-TestMessage</t>
+  </si>
+  <si>
+    <t>RFW-TransactionQueue</t>
   </si>
 </sst>
 </file>
@@ -685,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -858,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -880,6 +895,30 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>